<commit_message>
conteudo das aulas de PL
</commit_message>
<xml_diff>
--- a/notas_semestre_passado.xlsx
+++ b/notas_semestre_passado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Física</t>
+          <t>FÃ­sica</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Programação Orientada a Objetos</t>
+          <t>ProgramaÃ§Ã£o Orientada a Objetos</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -473,6 +473,26 @@
       </c>
       <c r="B4" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AnÃ¡lise de ModelaÃ§Ã£o de Software</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Armazenamento de Dados</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>